<commit_message>
fix index out of bound
</commit_message>
<xml_diff>
--- a/samples/templates/32readwriteAreaChart1.xlsx
+++ b/samples/templates/32readwriteAreaChart1.xlsx
@@ -1,15 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rounded\samples\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D2701F-BB4D-4A40-BAC2-CB253A891F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,15 +117,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -217,44 +238,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>540</c:v>
+                  <c:v>2690</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2520</c:v>
+                  <c:v>2680</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>740</c:v>
+                  <c:v>1470</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>530</c:v>
+                  <c:v>2820</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1710</c:v>
+                  <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2140</c:v>
+                  <c:v>2650</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3220</c:v>
+                  <c:v>1320</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1330</c:v>
+                  <c:v>1090</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>570</c:v>
+                  <c:v>2390</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1940</c:v>
+                  <c:v>2670</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1300</c:v>
+                  <c:v>2660</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2870</c:v>
+                  <c:v>2270</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4FB6-4236-8CE9-B34BDDA6CF3B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -337,7 +363,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -400,7 +432,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,9 +465,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,6 +517,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -643,19 +709,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
@@ -671,7 +737,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2">
         <v>2008</v>
@@ -692,7 +758,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -731,216 +797,216 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:M7" ca="1" si="0">(RANDBETWEEN(-50,250)+100)*10</f>
-        <v>2280</v>
+        <v>2560</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>1600</v>
+        <v>2300</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>2000</v>
+        <v>2960</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>2810</v>
+        <v>1560</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>920</v>
+        <v>890</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>3170</v>
+        <v>2380</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>1430</v>
+        <v>2920</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>2320</v>
+        <v>970</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>970</v>
+        <v>1450</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>2430</v>
+        <v>2020</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>3210</v>
+        <v>1920</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>3310</v>
+        <v>2450</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>660</v>
+        <v>1200</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>2910</v>
+        <v>630</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>780</v>
+        <v>1610</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>2740</v>
+        <v>570</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>2000</v>
+        <v>1470</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>1320</v>
+        <v>3120</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>1220</v>
+        <v>3000</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>3380</v>
+        <v>1300</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>1390</v>
+        <v>1350</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>3110</v>
+        <v>2040</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>3090</v>
+        <v>3120</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>2510</v>
+        <v>1100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>540</v>
+        <v>2690</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>2520</v>
+        <v>2680</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>740</v>
+        <v>1470</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>530</v>
+        <v>2820</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>1710</v>
+        <v>850</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>2140</v>
+        <v>2650</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>3220</v>
+        <v>1320</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>1330</v>
+        <v>1090</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>570</v>
+        <v>2390</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>1940</v>
+        <v>2670</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>1300</v>
+        <v>2660</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
-        <v>2870</v>
+        <v>2270</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>1620</v>
+        <v>2650</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>600</v>
+        <v>3450</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>640</v>
+        <v>2880</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>670</v>
+        <v>2550</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>3060</v>
+        <v>3400</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1320</v>
+        <v>830</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>1230</v>
+        <v>2630</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>1630</v>
+        <v>2640</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>3460</v>
+        <v>1160</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>3300</v>
+        <v>1470</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>1190</v>
+        <v>1460</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>2570</v>
+        <v>1910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>